<commit_message>
added const q model run
</commit_message>
<xml_diff>
--- a/assessments/yfs/DateTempTests.xlsx
+++ b/assessments/yfs/DateTempTests.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="33600" windowHeight="18440"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="33600" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="171027" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>$eb_bts</t>
   </si>
@@ -93,15 +93,18 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>Constant q</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -142,8 +145,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -460,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:P10"/>
+      <selection activeCell="F16" sqref="F16:W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -670,45 +673,43 @@
       <c r="B7">
         <v>2511.84</v>
       </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
+      <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3">
-        <v>1383.3</v>
+        <v>1396.02</v>
       </c>
       <c r="J7" s="3">
-        <v>85.284499999999994</v>
+        <v>108.339</v>
       </c>
       <c r="K7" s="4">
-        <v>0.152615</v>
+        <v>0.170124</v>
       </c>
       <c r="L7" s="3">
-        <v>634.23500000000001</v>
+        <v>621.17999999999995</v>
       </c>
       <c r="M7" s="3">
-        <v>568.27499999999998</v>
+        <v>572.85699999999997</v>
       </c>
       <c r="N7" s="3">
-        <v>24.87293</v>
+        <v>24.05059</v>
       </c>
       <c r="O7" s="3">
-        <v>67.381699999999995</v>
+        <v>65.866699999999994</v>
       </c>
       <c r="P7" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Q7" s="3">
         <f>I7-SUM(J7:O7)+S7</f>
-        <v>3.3458710000001082</v>
+        <v>3.8239999999999248</v>
       </c>
       <c r="R7" s="3">
         <v>0</v>
       </c>
       <c r="S7" s="3">
-        <v>0.247616</v>
+        <v>0.26741399999999999</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="24">
@@ -718,45 +719,43 @@
       <c r="B8">
         <v>2180.75</v>
       </c>
-      <c r="G8" s="1">
-        <v>2</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="3">
-        <v>1371.04</v>
+        <v>1383.3</v>
       </c>
       <c r="J8" s="3">
-        <v>91.868899999999996</v>
+        <v>85.284499999999994</v>
       </c>
       <c r="K8" s="4">
-        <v>0.16231799999999999</v>
+        <v>0.152615</v>
       </c>
       <c r="L8" s="3">
-        <v>615.43899999999996</v>
+        <v>634.23500000000001</v>
       </c>
       <c r="M8" s="3">
-        <v>570.97400000000005</v>
+        <v>568.27499999999998</v>
       </c>
       <c r="N8" s="3">
-        <v>24.587820000000001</v>
+        <v>24.87293</v>
       </c>
       <c r="O8" s="3">
-        <v>64.762200000000007</v>
+        <v>67.381699999999995</v>
       </c>
       <c r="P8" s="2">
         <v>488</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" ref="Q8:Q10" si="0">I8-SUM(J8:O8)+S8</f>
-        <v>3.5438940000000132</v>
+        <f>I8-SUM(J8:O8)+S8</f>
+        <v>3.3458710000001082</v>
       </c>
       <c r="R8" s="3">
         <v>0</v>
       </c>
       <c r="S8" s="3">
-        <v>0.29813200000000001</v>
+        <v>0.247616</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="24">
@@ -766,46 +765,43 @@
       <c r="B9">
         <v>2313.62</v>
       </c>
-      <c r="G9" s="1">
-        <v>3</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I9" s="3">
-        <v>1365.58</v>
+        <v>1371.04</v>
       </c>
       <c r="J9" s="3">
-        <v>73.977800000000002</v>
+        <v>91.868899999999996</v>
       </c>
       <c r="K9" s="4">
-        <v>0.14599500000000001</v>
+        <v>0.16231799999999999</v>
       </c>
       <c r="L9" s="3">
-        <v>626.34100000000001</v>
+        <v>615.43899999999996</v>
       </c>
       <c r="M9" s="3">
-        <v>567.96400000000006</v>
+        <v>570.97400000000005</v>
       </c>
       <c r="N9" s="3">
-        <v>26.83145</v>
+        <v>24.587820000000001</v>
       </c>
       <c r="O9" s="3">
-        <v>67.923100000000005</v>
+        <v>64.762200000000007</v>
       </c>
       <c r="P9" s="2">
-        <f>P8+1</f>
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="0"/>
-        <v>2.5765160000000096</v>
+        <f t="shared" ref="Q9:Q11" si="0">I9-SUM(J9:O9)+S9</f>
+        <v>3.5438940000000132</v>
       </c>
       <c r="R9" s="3">
         <v>0</v>
       </c>
       <c r="S9" s="3">
-        <v>0.17986099999999999</v>
+        <v>0.29813200000000001</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="24">
@@ -815,46 +811,44 @@
       <c r="B10">
         <v>2179.61</v>
       </c>
-      <c r="G10" s="1">
-        <v>4</v>
-      </c>
+      <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I10" s="3">
-        <v>1357.29</v>
+        <v>1365.58</v>
       </c>
       <c r="J10" s="3">
-        <v>72.5655</v>
+        <v>73.977800000000002</v>
       </c>
       <c r="K10" s="4">
-        <v>0.143981</v>
+        <v>0.14599500000000001</v>
       </c>
       <c r="L10" s="3">
-        <v>617.76199999999994</v>
+        <v>626.34100000000001</v>
       </c>
       <c r="M10" s="3">
-        <v>567.92399999999998</v>
+        <v>567.96400000000006</v>
       </c>
       <c r="N10" s="3">
-        <v>25.329280000000001</v>
+        <v>26.83145</v>
       </c>
       <c r="O10" s="3">
-        <v>70.207599999999999</v>
+        <v>67.923100000000005</v>
       </c>
       <c r="P10" s="2">
         <f>P9+1</f>
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="Q10" s="3">
         <f t="shared" si="0"/>
-        <v>4.1612840000000633</v>
+        <v>2.5765160000000096</v>
       </c>
       <c r="R10" s="3">
         <v>0</v>
       </c>
       <c r="S10" s="3">
-        <v>0.80364500000000005</v>
+        <v>0.17986099999999999</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="24">
@@ -865,6 +859,44 @@
         <v>2391.86</v>
       </c>
       <c r="G11" s="1"/>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1357.29</v>
+      </c>
+      <c r="J11" s="3">
+        <v>72.5655</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.143981</v>
+      </c>
+      <c r="L11" s="3">
+        <v>617.76199999999994</v>
+      </c>
+      <c r="M11" s="3">
+        <v>567.92399999999998</v>
+      </c>
+      <c r="N11" s="3">
+        <v>25.329280000000001</v>
+      </c>
+      <c r="O11" s="3">
+        <v>70.207599999999999</v>
+      </c>
+      <c r="P11" s="2">
+        <f>P10+1</f>
+        <v>490</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1612840000000633</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0.80364500000000005</v>
+      </c>
     </row>
     <row r="12" spans="1:38" ht="24">
       <c r="A12">
@@ -873,9 +905,7 @@
       <c r="B12">
         <v>2201.52</v>
       </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:38" ht="24">
       <c r="A13">
@@ -884,9 +914,7 @@
       <c r="B13">
         <v>2468.4299999999998</v>
       </c>
-      <c r="G13" s="1">
-        <v>2</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:38" ht="24">
       <c r="A14">
@@ -895,9 +923,7 @@
       <c r="B14">
         <v>2597.19</v>
       </c>
-      <c r="G14" s="1">
-        <v>3</v>
-      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:38" ht="24">
       <c r="A15">
@@ -906,9 +932,7 @@
       <c r="B15">
         <v>2012.4</v>
       </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:38">
       <c r="A16">

</xml_diff>